<commit_message>
chore: add network output for network examples
</commit_message>
<xml_diff>
--- a/examples/data/hazard_overlay/reference/static/output_graph/hazard_names.xlsx
+++ b/examples/data/hazard_overlay/reference/static/output_graph/hazard_names.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>data\hazard_overlay\hazard\max_flood_depth.tif</t>
+          <t>data/hazard_overlay/hazard/max_flood_depth.tif</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>data\hazard_overlay\hazard\max_flood_depth.tif</t>
+          <t>data/hazard_overlay/hazard/max_flood_depth.tif</t>
         </is>
       </c>
     </row>

</xml_diff>